<commit_message>
Primeiro commit do branch do projeto do modulo 02
</commit_message>
<xml_diff>
--- a/Docs/Project/taskboard.xlsx
+++ b/Docs/Project/taskboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BZ241WX\Documents\InfNet\CursoPosDataScience\mit_ds_course\Docs\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564516F2-79BB-499C-B441-2363D0572C60}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87678075-BDEB-498D-9070-B646C42F42D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EFC1725C-2304-4691-9531-9BACDA3C9584}"/>
   </bookViews>
@@ -303,13 +303,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{64C095BF-52B4-4D2B-B569-688493D01887}" name="Table1" displayName="Table1" ref="A1:H12" totalsRowShown="0" dataDxfId="8">
-  <autoFilter ref="A1:H12" xr:uid="{8F24B1FF-F8FC-45B9-9C3C-70CF193FBC52}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H12" xr:uid="{8F24B1FF-F8FC-45B9-9C3C-70CF193FBC52}"/>
   <tableColumns count="8">
     <tableColumn id="9" xr3:uid="{12F19273-FB4D-4151-BD67-9A0F6235ACFD}" name="ID" dataDxfId="7"/>
     <tableColumn id="1" xr3:uid="{6F22CA81-2B39-452D-9511-688464A1750E}" name="Story" dataDxfId="6"/>
@@ -623,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC68CFBD-2DA0-4910-875F-F7F64F0C64ED}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -816,7 +810,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -842,7 +836,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="159.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -868,7 +862,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -894,7 +888,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -920,7 +914,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>

</xml_diff>